<commit_message>
one more chart added
</commit_message>
<xml_diff>
--- a/cardatabase.xlsx.xlsx
+++ b/cardatabase.xlsx.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15369ddf0b8636d1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imran\OneDrive\Desktop\Excel_learning_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC142D9E-31AB-432A-BB67-52748F02F15F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{DC142D9E-31AB-432A-BB67-52748F02F15F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0D0D4475-476A-42E3-B08A-C6559A734FD0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
     <sheet name="car inventory" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,8 +953,2423 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[cardatabase.xlsx.xlsx]pivot!PivotTable1</c:name>
+    <c:fmtId val="2"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pivot!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>pivot!$A$4:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>Bard</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ewenty</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gaul</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Howard</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hulinski</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jones</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lyon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>McCall</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Praulty</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Rodriguez</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Santos</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Smith</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Swartz</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Torrens</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Vizzini</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Yousef</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pivot!$B$4:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>144647.69999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35995.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154427.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>179986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>143640.70000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55657.600000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107450.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>127731.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70964.899999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65315</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56187.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>141229.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305432.40000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>177713.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65964.899999999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>130601.59999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19341.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C470-4E68-873C-F354A14A2411}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="102459648"/>
+        <c:axId val="101787536"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="102459648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101787536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="101787536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102459648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'car inventory'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Miles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'car inventory'!$G$2:$G$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'car inventory'!$H$2:$H$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>40326.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44974.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44946.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37558.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36438.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46311.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52229.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27637.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27534.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19341.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22521.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13682.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28464.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19421.099999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14289.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31144.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>83162.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>80685.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>114660.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>93382.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>85928</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>67829.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48114.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>64467.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>73444.399999999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17556.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29601.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22128.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>82374</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69891.899999999994</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>22573</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33477.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>30555.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24513.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13867.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>60389.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50854.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42504.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>68658.899999999994</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3708.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>64542</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42074.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>27394.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>79420.600000000006</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>77243.100000000006</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>72527.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>52699.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29102.3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>22282</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20223.900000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>22188.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-72A3-4DC4-84EE-583258E3BA83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="196930976"/>
+        <c:axId val="103756752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="196930976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>AGE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103756752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="103756752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Miles</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> Driven</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="196930976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28ACC898-56D4-4306-BB28-F0B9ED29AFC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>403860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{803EECF9-4800-4796-B740-88F7D2C1CD51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ali Imran Adil" refreshedDate="45376.354176851855" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="52">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ali Imran Adil" refreshedDate="45376.354176851855" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="52" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N53" sheet="car inventory"/>
   </cacheSource>
@@ -1880,7 +4295,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -2010,6 +4425,17 @@
   <dataFields count="1">
     <dataField name="Sum of Miles" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2318,11 +4744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2494,15 +4920,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N53"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5442,5 +7869,6 @@
     <sortCondition ref="D57:D67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>